<commit_message>
added Sarima Model for Karnataka
</commit_message>
<xml_diff>
--- a/Karnataka/Future_Predicted_KA.xlsx
+++ b/Karnataka/Future_Predicted_KA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karti\Desktop\Arima &amp; Sarima - COVID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karti\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{FAFDB4A9-5870-47ED-9AC1-8B3F163D5118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{EA2AD6AF-43D0-4997-8EF8-ADCDD9C3F83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,22 +171,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>87081</xdr:rowOff>
+      <xdr:colOff>613837</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C532F7-617F-44A2-B024-A5684E491C88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{463179D9-33D6-4E84-9773-3E93A38488B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -202,8 +202,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="99060" y="4770120"/>
-          <a:ext cx="6903720" cy="4537161"/>
+          <a:off x="38100" y="4709161"/>
+          <a:ext cx="7136557" cy="4747260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -215,22 +215,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
+      <xdr:colOff>617221</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>53341</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>134632</xdr:rowOff>
+      <xdr:colOff>515849</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>99059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BB2FFE7-56A2-4CC4-A787-A2F0EE68B481}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{569F19EE-9074-474B-8D37-14C68F80DE23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -246,8 +246,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7018021" y="4747261"/>
-          <a:ext cx="6896099" cy="4607571"/>
+          <a:off x="7178041" y="4739640"/>
+          <a:ext cx="7030948" cy="4747259"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -259,22 +259,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>876301</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>137161</xdr:rowOff>
+      <xdr:colOff>1188721</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102454</xdr:colOff>
+      <xdr:colOff>272660</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46719331-DB94-4946-8659-D655A2AA19F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9862C98-1E6A-4E78-ACAC-9D30697528B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -290,8 +290,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3268981" y="9357361"/>
-          <a:ext cx="7356693" cy="4975859"/>
+          <a:off x="3581401" y="9509760"/>
+          <a:ext cx="7214479" cy="4762500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -631,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>671.08097130962301</v>
+        <v>739.02741706859797</v>
       </c>
       <c r="C2">
-        <v>454.12922446759598</v>
+        <v>389.57660453124703</v>
       </c>
       <c r="D2">
-        <v>3.6836433710546701</v>
+        <v>13.219007470484099</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>651.04836106165897</v>
+        <v>717.83525831691395</v>
       </c>
       <c r="C3">
-        <v>364.382675314621</v>
+        <v>372.65968991954702</v>
       </c>
       <c r="D3">
-        <v>4.5456559042031</v>
+        <v>15.994200010758</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,13 +659,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>377.51409883219799</v>
+        <v>730.68780508265002</v>
       </c>
       <c r="C4">
-        <v>452.74528073973698</v>
+        <v>449.78355782223503</v>
       </c>
       <c r="D4">
-        <v>4.5356171908778302</v>
+        <v>13.931531607394501</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>612.18170263891602</v>
+        <v>829.37314893212397</v>
       </c>
       <c r="C5">
-        <v>405.69572544418003</v>
+        <v>333.05901951106301</v>
       </c>
       <c r="D5">
-        <v>5.9134164218208802</v>
+        <v>14.279018679689401</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,13 +687,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>278.708063138444</v>
+        <v>821.80175338903905</v>
       </c>
       <c r="C6">
-        <v>410.95560025748898</v>
+        <v>454.96394244469099</v>
       </c>
       <c r="D6">
-        <v>3.99838200103187</v>
+        <v>11.9019158883447</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,13 +701,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>413.41484338745101</v>
+        <v>798.91576861513499</v>
       </c>
       <c r="C7">
-        <v>531.51815739184997</v>
+        <v>347.46475785040701</v>
       </c>
       <c r="D7">
-        <v>4.8604116318743804</v>
+        <v>13.027993490452801</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,13 +715,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>381.91777216808401</v>
+        <v>812.922048733765</v>
       </c>
       <c r="C8">
-        <v>469.95051829453399</v>
+        <v>645.69004400566996</v>
       </c>
       <c r="D8">
-        <v>4.8503741535320204</v>
+        <v>13.6379738712522</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,13 +729,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>419.054784157835</v>
+        <v>916.38074977438305</v>
       </c>
       <c r="C9">
-        <v>572.03497728236198</v>
+        <v>521.58108121377404</v>
       </c>
       <c r="D9">
-        <v>6.2281027868316796</v>
+        <v>17.987660037800701</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +743,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>726.65403025437399</v>
+        <v>908.83625472502501</v>
       </c>
       <c r="C10">
-        <v>520.74194955769894</v>
+        <v>512.99268005200497</v>
       </c>
       <c r="D10">
-        <v>4.3130397180045801</v>
+        <v>12.0823966513044</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,13 +757,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>691.83743823746795</v>
+        <v>884.25591350400896</v>
       </c>
       <c r="C11">
-        <v>538.23556293289698</v>
+        <v>460.26009746638499</v>
       </c>
       <c r="D11">
-        <v>5.1750647804333099</v>
+        <v>15.9056069998417</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +771,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>389.63816236744401</v>
+        <v>899.45319457135997</v>
       </c>
       <c r="C12">
-        <v>438.347539656018</v>
+        <v>473.54595415178198</v>
       </c>
       <c r="D12">
-        <v>5.1650269721100299</v>
+        <v>16.0593928007617</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,13 +785,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>638.42184328029805</v>
+        <v>1007.72071775428</v>
       </c>
       <c r="C13">
-        <v>534.745675646888</v>
+        <v>553.168868331932</v>
       </c>
       <c r="D13">
-        <v>6.5427744687280196</v>
+        <v>18.538903333119901</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,13 +799,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>275.93213704435698</v>
+        <v>1000.22898257587</v>
       </c>
       <c r="C14">
-        <v>481.35603501426198</v>
+        <v>445.90092776215198</v>
       </c>
       <c r="D14">
-        <v>4.6277190545057501</v>
+        <v>16.707505090045402</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +813,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>419.90826993306501</v>
+        <v>973.95410223554404</v>
       </c>
       <c r="C15">
-        <v>490.97417561774103</v>
+        <v>541.06775336741896</v>
       </c>
       <c r="D15">
-        <v>5.4897453375905796</v>
+        <v>17.1405536008761</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,13 +827,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>388.31270985075099</v>
+        <v>990.38017828909597</v>
       </c>
       <c r="C16">
-        <v>601.76288008652602</v>
+        <v>447.86684845466999</v>
       </c>
       <c r="D16">
-        <v>5.4797076174364596</v>
+        <v>15.1620965037036</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,13 +841,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>426.95424678391998</v>
+        <v>1103.4925967211</v>
       </c>
       <c r="C17">
-        <v>547.76797421361402</v>
+        <v>708.47673976131</v>
       </c>
       <c r="D17">
-        <v>6.8574500738751798</v>
+        <v>16.564760408365402</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,13 +855,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>765.73580058268203</v>
+        <v>1096.08012787812</v>
       </c>
       <c r="C18">
-        <v>643.78322389685297</v>
+        <v>618.79613872777895</v>
       </c>
       <c r="D18">
-        <v>4.9423926143828298</v>
+        <v>16.587726881916499</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,13 +869,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>719.55309309703205</v>
+        <v>1068.11120856313</v>
       </c>
       <c r="C19">
-        <v>603.84984131722103</v>
+        <v>576.26131545971305</v>
       </c>
       <c r="D19">
-        <v>5.8044185713147796</v>
+        <v>20.532077757113701</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,13 +883,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>392.792621454901</v>
+        <v>1085.8045247688401</v>
       </c>
       <c r="C20">
-        <v>612.20992692619495</v>
+        <v>546.93611140256496</v>
       </c>
       <c r="D20">
-        <v>5.7943808276023301</v>
+        <v>15.141305352707001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,13 +897,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>654.79993514963405</v>
+        <v>1203.7985658625801</v>
       </c>
       <c r="C21">
-        <v>517.57660477464799</v>
+        <v>545.38743807657897</v>
       </c>
       <c r="D21">
-        <v>7.1721246307503899</v>
+        <v>19.0161200443345</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,13 +911,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>267.00015127215403</v>
+        <v>1196.4925337355601</v>
       </c>
       <c r="C22">
-        <v>609.81122402861797</v>
+        <v>623.966160129728</v>
       </c>
       <c r="D22">
-        <v>5.2570677177434302</v>
+        <v>19.226769406480901</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,13 +925,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>419.742398280727</v>
+        <v>1166.8307642720999</v>
       </c>
       <c r="C23">
-        <v>559.70661709481999</v>
+        <v>511.98892216632601</v>
       </c>
       <c r="D23">
-        <v>6.1190937618217101</v>
+        <v>21.820938001945901</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,13 +939,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>387.58980920716101</v>
+        <v>1185.8304187393101</v>
       </c>
       <c r="C24">
-        <v>567.06657146166106</v>
+        <v>620.20477323134503</v>
       </c>
       <c r="D24">
-        <v>6.1090560244039303</v>
+        <v>19.899858993984601</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,13 +953,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>428.050626365825</v>
+        <v>1308.74346450245</v>
       </c>
       <c r="C25">
-        <v>682.91934871037904</v>
+        <v>519.99994005513804</v>
       </c>
       <c r="D25">
-        <v>7.4867994677183498</v>
+        <v>20.2997289259485</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +967,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>793.96706915479297</v>
+        <v>1301.57170309977</v>
       </c>
       <c r="C26">
-        <v>625.00082624382003</v>
+        <v>798.88644067577502</v>
       </c>
       <c r="D26">
-        <v>5.5717424086933702</v>
+        <v>18.166687031811598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>